<commit_message>
Updating Advanced Book Search for validation with Excel data
</commit_message>
<xml_diff>
--- a/Sprint_2/src/test/resources/data/AdvancedBookSearchData.xlsx
+++ b/Sprint_2/src/test/resources/data/AdvancedBookSearchData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\New_Script\Sprint-2\Sprint_2\src\test\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Esha\git\Sprint-2\Sprint_2\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D42C0AE0-F3D4-4514-8515-A78C84B8B636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E3D9A6-5106-4E4E-B4E8-787D13ECE61F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{405FAE42-A142-41FD-ADE6-8DF950D69CD0}"/>
   </bookViews>
@@ -20,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>Author</t>
   </si>
@@ -132,11 +123,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -457,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B50DC717-02F5-4040-9A7C-D7E2913D0EDA}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -469,13 +457,11 @@
     <col min="2" max="2" width="11.6640625" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="14.88671875" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
-    <col min="8" max="8" width="11.44140625" customWidth="1"/>
+    <col min="5" max="5" width="13.21875" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -494,87 +480,65 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>1</v>
-      </c>
     </row>
-    <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="3"/>
-      <c r="G4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>